<commit_message>
Little Bit of Update
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -619,7 +619,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="7">
-        <v>44743</v>
+        <v>44774</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>72</v>
@@ -741,7 +741,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="7">
-        <v>44749</v>
+        <v>44780</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>73</v>

</xml_diff>